<commit_message>
Changed how jobs get executed
</commit_message>
<xml_diff>
--- a/test/HWDBUtility/SystemTest/003/Biff-SN-errors.xlsx
+++ b/test/HWDBUtility/SystemTest/003/Biff-SN-errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alexwagner\Projects\DUNE-HWDB-Python\test\HWDBUtility\SystemTest\003\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1CE7D4-A16E-4DC4-9FDF-02F88E8D9510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98A0119-84C4-4D19-856D-21BFE3D24654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19932" yWindow="1452" windowWidth="19644" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21192" yWindow="756" windowWidth="19644" windowHeight="11004" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biff-Items" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Record Type</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>conflicts with several items</t>
+  </si>
+  <si>
+    <t>Z00100300022-00044</t>
+  </si>
+  <si>
+    <t>changing to SN that another item is also trying to claim</t>
   </si>
 </sst>
 </file>
@@ -563,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,6 +804,17 @@
       </c>
       <c r="E14" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>